<commit_message>
Added more headers to BOM
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/2014_08_14/BOM.xlsx
+++ b/PCB Design/Fabrication/2014_08_14/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Fabrication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Fabrication\2014_08_14\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -610,7 +610,7 @@
     <t>568-5931-1-ND </t>
   </si>
   <si>
-    <t>609-3485-1-N, A30848-ND, A31115-ND</t>
+    <t>609-3485-1-N, A30848-ND, A31115-ND, A31113-ND , 29400E-01-20-ND</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2117,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added female headers for Teensy to BOM
</commit_message>
<xml_diff>
--- a/PCB Design/Fabrication/2014_08_14/BOM.xlsx
+++ b/PCB Design/Fabrication/2014_08_14/BOM.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="166">
   <si>
     <t>Qty</t>
   </si>
@@ -595,9 +595,6 @@
     <t>U$2</t>
   </si>
   <si>
-    <t>Footprint for Teensy 3.1 board using all pads and all through-holes. Pads need a 2x7 0.1 SMD header."</t>
-  </si>
-  <si>
     <t>2N7002KCT-ND</t>
   </si>
   <si>
@@ -611,6 +608,15 @@
   </si>
   <si>
     <t>609-3485-1-N, A30848-ND, A31115-ND, A31113-ND , 29400E-01-20-ND</t>
+  </si>
+  <si>
+    <t>Male pins on the Teensy board</t>
+  </si>
+  <si>
+    <t>Female pins for the Teensy board</t>
+  </si>
+  <si>
+    <t>S7005-ND, S7036-ND, S6100-ND</t>
   </si>
 </sst>
 </file>
@@ -2114,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,7 +2180,7 @@
         <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2441,7 +2447,7 @@
         <v>149</v>
       </c>
       <c r="G14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2464,7 +2470,7 @@
         <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,7 +2493,7 @@
         <v>152</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2541,22 +2547,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>157</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>163</v>
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2564,22 +2570,30 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
+        <v>163</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>